<commit_message>
atualização de nomes de distribuiodoras incluindo equatorial GO
</commit_message>
<xml_diff>
--- a/inst/dados_premissas/2022/consumidores_a.xlsx
+++ b/inst/dados_premissas/2022/consumidores_a.xlsx
@@ -1,21 +1,227 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Arquivos Locais\projetos\epe4md-git3\inst\dados_premissas\2022\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A0C394-D87C-4902-9142-0FAA6B2F4A18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+  <si>
+    <t>nome_4md</t>
+  </si>
+  <si>
+    <t>2013</t>
+  </si>
+  <si>
+    <t>2014</t>
+  </si>
+  <si>
+    <t>2015</t>
+  </si>
+  <si>
+    <t>2016</t>
+  </si>
+  <si>
+    <t>2017</t>
+  </si>
+  <si>
+    <t>2018</t>
+  </si>
+  <si>
+    <t>2019</t>
+  </si>
+  <si>
+    <t>2020</t>
+  </si>
+  <si>
+    <t>2021</t>
+  </si>
+  <si>
+    <t>2022</t>
+  </si>
+  <si>
+    <t>AME</t>
+  </si>
+  <si>
+    <t>CEA</t>
+  </si>
+  <si>
+    <t>CEB</t>
+  </si>
+  <si>
+    <t>CEEE</t>
+  </si>
+  <si>
+    <t>CELESC</t>
+  </si>
+  <si>
+    <t>CELPE</t>
+  </si>
+  <si>
+    <t>CEMIG</t>
+  </si>
+  <si>
+    <t>CHESP</t>
+  </si>
+  <si>
+    <t>COCEL</t>
+  </si>
+  <si>
+    <t>COELBA</t>
+  </si>
+  <si>
+    <t>COOPERALIANÇA</t>
+  </si>
+  <si>
+    <t>COPEL</t>
+  </si>
+  <si>
+    <t>COSERN</t>
+  </si>
+  <si>
+    <t>CPFL PAULISTA</t>
+  </si>
+  <si>
+    <t>CPFL PIRATININGA</t>
+  </si>
+  <si>
+    <t>CPFL SANTA CRUZ</t>
+  </si>
+  <si>
+    <t>DCELT</t>
+  </si>
+  <si>
+    <t>DEMEI</t>
+  </si>
+  <si>
+    <t>DMED</t>
+  </si>
+  <si>
+    <t>EAC</t>
+  </si>
+  <si>
+    <t>EBO</t>
+  </si>
+  <si>
+    <t>EDP ES</t>
+  </si>
+  <si>
+    <t>EDP SP</t>
+  </si>
+  <si>
+    <t>EFLJC</t>
+  </si>
+  <si>
+    <t>EFLUL</t>
+  </si>
+  <si>
+    <t>ELEKTRO</t>
+  </si>
+  <si>
+    <t>ELETROCAR</t>
+  </si>
+  <si>
+    <t>ELFSM</t>
+  </si>
+  <si>
+    <t>EMG</t>
+  </si>
+  <si>
+    <t>EMS</t>
+  </si>
+  <si>
+    <t>EMT</t>
+  </si>
+  <si>
+    <t>ENEL CE</t>
+  </si>
+  <si>
+    <t>ENEL RJ</t>
+  </si>
+  <si>
+    <t>ENEL SP</t>
+  </si>
+  <si>
+    <t>ENF</t>
+  </si>
+  <si>
+    <t>EPB</t>
+  </si>
+  <si>
+    <t>EQUATORIAL AL</t>
+  </si>
+  <si>
+    <t>EQUATORIAL MA</t>
+  </si>
+  <si>
+    <t>EQUATORIAL PA</t>
+  </si>
+  <si>
+    <t>EQUATORIAL PI</t>
+  </si>
+  <si>
+    <t>ERO</t>
+  </si>
+  <si>
+    <t>ESE</t>
+  </si>
+  <si>
+    <t>ESS</t>
+  </si>
+  <si>
+    <t>ETO</t>
+  </si>
+  <si>
+    <t>FORCEL</t>
+  </si>
+  <si>
+    <t>HIDROPAN</t>
+  </si>
+  <si>
+    <t>LIGHT</t>
+  </si>
+  <si>
+    <t>MUXENERGIA</t>
+  </si>
+  <si>
+    <t>OUTRA</t>
+  </si>
+  <si>
+    <t>RGE</t>
+  </si>
+  <si>
+    <t>RORAIMA</t>
+  </si>
+  <si>
+    <t>SULGIPE</t>
+  </si>
+  <si>
+    <t>UHENPAL</t>
+  </si>
+  <si>
+    <t>EQUATORIAL GO</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,11 +269,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -109,7 +323,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -141,9 +355,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -175,6 +407,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -350,75 +600,51 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>nome_4md</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>2013</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>2014</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>2015</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>2016</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>2017</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>2018</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>2019</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>AME</t>
-        </is>
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>11</v>
       </c>
       <c r="B2">
         <v>2726</v>
@@ -451,11 +677,9 @@
         <v>2767</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>CEA</t>
-        </is>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>12</v>
       </c>
       <c r="B3">
         <v>546</v>
@@ -488,11 +712,9 @@
         <v>652</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>CEB</t>
-        </is>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>13</v>
       </c>
       <c r="B4">
         <v>2141</v>
@@ -525,11 +747,9 @@
         <v>2398</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>CEEE</t>
-        </is>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>14</v>
       </c>
       <c r="B5">
         <v>5327</v>
@@ -562,11 +782,9 @@
         <v>4546</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>CELESC</t>
-        </is>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>15</v>
       </c>
       <c r="B6">
         <v>9782</v>
@@ -599,11 +817,9 @@
         <v>8957</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>CELPE</t>
-        </is>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>16</v>
       </c>
       <c r="B7">
         <v>5679</v>
@@ -636,11 +852,9 @@
         <v>5518</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>CEMIG</t>
-        </is>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>17</v>
       </c>
       <c r="B8">
         <v>12973</v>
@@ -673,11 +887,9 @@
         <v>13459</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>CHESP</t>
-        </is>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>18</v>
       </c>
       <c r="B9">
         <v>50</v>
@@ -710,11 +922,9 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>COCEL</t>
-        </is>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>19</v>
       </c>
       <c r="B10">
         <v>166</v>
@@ -747,11 +957,9 @@
         <v>183</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>COELBA</t>
-        </is>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>20</v>
       </c>
       <c r="B11">
         <v>7950</v>
@@ -784,11 +992,9 @@
         <v>8163</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>COOPERALIANÇA</t>
-        </is>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>21</v>
       </c>
       <c r="B12">
         <v>114</v>
@@ -821,11 +1027,9 @@
         <v>96</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>COPEL</t>
-        </is>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>22</v>
       </c>
       <c r="B13">
         <v>13438</v>
@@ -858,11 +1062,9 @@
         <v>13149</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>COSERN</t>
-        </is>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>23</v>
       </c>
       <c r="B14">
         <v>2648</v>
@@ -895,11 +1097,9 @@
         <v>2484</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>CPFL PAULISTA</t>
-        </is>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>24</v>
       </c>
       <c r="B15">
         <v>14842</v>
@@ -932,11 +1132,9 @@
         <v>12758</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>CPFL PIRATININGA</t>
-        </is>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>25</v>
       </c>
       <c r="B16">
         <v>4450</v>
@@ -969,11 +1167,9 @@
         <v>4743</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>CPFL SANTA CRUZ</t>
-        </is>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>26</v>
       </c>
       <c r="B17">
         <v>1423</v>
@@ -1006,11 +1202,9 @@
         <v>1548</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>DCELT</t>
-        </is>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>27</v>
       </c>
       <c r="B18">
         <v>144</v>
@@ -1043,11 +1237,9 @@
         <v>158</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>DEMEI</t>
-        </is>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>28</v>
       </c>
       <c r="B19">
         <v>88</v>
@@ -1080,11 +1272,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>DMED</t>
-        </is>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>29</v>
       </c>
       <c r="B20">
         <v>169</v>
@@ -1117,11 +1307,9 @@
         <v>158</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>EAC</t>
-        </is>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>30</v>
       </c>
       <c r="B21">
         <v>428</v>
@@ -1154,11 +1342,9 @@
         <v>753</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>EBO</t>
-        </is>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>31</v>
       </c>
       <c r="B22">
         <v>342</v>
@@ -1191,11 +1377,9 @@
         <v>362</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>EDP ES</t>
-        </is>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>32</v>
       </c>
       <c r="B23">
         <v>3199</v>
@@ -1228,11 +1412,9 @@
         <v>2816</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>EDP SP</t>
-        </is>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>33</v>
       </c>
       <c r="B24">
         <v>4078</v>
@@ -1265,11 +1447,9 @@
         <v>3732</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>EFLJC</t>
-        </is>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>34</v>
       </c>
       <c r="B25">
         <v>13</v>
@@ -1302,11 +1482,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>EFLUL</t>
-        </is>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>35</v>
       </c>
       <c r="B26">
         <v>34</v>
@@ -1339,11 +1517,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>ELEKTRO</t>
-        </is>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>36</v>
       </c>
       <c r="B27">
         <v>6774</v>
@@ -1376,11 +1552,9 @@
         <v>6365</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>ELETROCAR</t>
-        </is>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>37</v>
       </c>
       <c r="B28">
         <v>118</v>
@@ -1413,11 +1587,9 @@
         <v>135</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>ELFSM</t>
-        </is>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>38</v>
       </c>
       <c r="B29">
         <v>213</v>
@@ -1450,11 +1622,9 @@
         <v>189</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>EMG</t>
-        </is>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>39</v>
       </c>
       <c r="B30">
         <v>498</v>
@@ -1487,11 +1657,9 @@
         <v>457</v>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>EMS</t>
-        </is>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>40</v>
       </c>
       <c r="B31">
         <v>3011</v>
@@ -1524,11 +1692,9 @@
         <v>3039</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>EMT</t>
-        </is>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>41</v>
       </c>
       <c r="B32">
         <v>4250</v>
@@ -1561,11 +1727,9 @@
         <v>5448</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>ENEL CE</t>
-        </is>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>42</v>
       </c>
       <c r="B33">
         <v>6444</v>
@@ -1598,11 +1762,9 @@
         <v>6857</v>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>ENEL GO</t>
-        </is>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>64</v>
       </c>
       <c r="B34">
         <v>7904</v>
@@ -1635,11 +1797,9 @@
         <v>7950</v>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>ENEL RJ</t>
-        </is>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>43</v>
       </c>
       <c r="B35">
         <v>5209</v>
@@ -1672,11 +1832,9 @@
         <v>5547</v>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>ENEL SP</t>
-        </is>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>44</v>
       </c>
       <c r="B36">
         <v>12952</v>
@@ -1709,11 +1867,9 @@
         <v>11056</v>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>ENF</t>
-        </is>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>45</v>
       </c>
       <c r="B37">
         <v>152</v>
@@ -1746,11 +1902,9 @@
         <v>142</v>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>EPB</t>
-        </is>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>46</v>
       </c>
       <c r="B38">
         <v>1581</v>
@@ -1783,11 +1937,9 @@
         <v>1748</v>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>EQUATORIAL AL</t>
-        </is>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>47</v>
       </c>
       <c r="B39">
         <v>2150</v>
@@ -1820,11 +1972,9 @@
         <v>2157</v>
       </c>
     </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>EQUATORIAL MA</t>
-        </is>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>48</v>
       </c>
       <c r="B40">
         <v>2250</v>
@@ -1857,11 +2007,9 @@
         <v>3001</v>
       </c>
     </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>EQUATORIAL PA</t>
-        </is>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>49</v>
       </c>
       <c r="B41">
         <v>4061</v>
@@ -1894,11 +2042,9 @@
         <v>4400</v>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>EQUATORIAL PI</t>
-        </is>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>50</v>
       </c>
       <c r="B42">
         <v>1728</v>
@@ -1931,11 +2077,9 @@
         <v>1926</v>
       </c>
     </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>ERO</t>
-        </is>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>51</v>
       </c>
       <c r="B43">
         <v>2039</v>
@@ -1968,11 +2112,9 @@
         <v>2219</v>
       </c>
     </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>ESE</t>
-        </is>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>52</v>
       </c>
       <c r="B44">
         <v>1223</v>
@@ -2005,11 +2147,9 @@
         <v>1172</v>
       </c>
     </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>ESS</t>
-        </is>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>53</v>
       </c>
       <c r="B45">
         <v>1869</v>
@@ -2042,11 +2182,9 @@
         <v>1957</v>
       </c>
     </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>ETO</t>
-        </is>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>54</v>
       </c>
       <c r="B46">
         <v>1092</v>
@@ -2079,11 +2217,9 @@
         <v>1268</v>
       </c>
     </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>FORCEL</t>
-        </is>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>55</v>
       </c>
       <c r="B47">
         <v>23</v>
@@ -2116,11 +2252,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>HIDROPAN</t>
-        </is>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>56</v>
       </c>
       <c r="B48">
         <v>72</v>
@@ -2153,11 +2287,9 @@
         <v>74</v>
       </c>
     </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>LIGHT</t>
-        </is>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>57</v>
       </c>
       <c r="B49">
         <v>6950</v>
@@ -2190,11 +2322,9 @@
         <v>4646</v>
       </c>
     </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>MUXENERGIA</t>
-        </is>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>58</v>
       </c>
       <c r="B50">
         <v>26</v>
@@ -2227,11 +2357,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>OUTRA</t>
-        </is>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>59</v>
       </c>
       <c r="B51">
         <v>1692</v>
@@ -2264,11 +2392,9 @@
         <v>2984</v>
       </c>
     </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>RGE</t>
-        </is>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>60</v>
       </c>
       <c r="B52">
         <v>12282</v>
@@ -2301,11 +2427,9 @@
         <v>11259</v>
       </c>
     </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>RORAIMA</t>
-        </is>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>61</v>
       </c>
       <c r="B53">
         <v>543</v>
@@ -2338,11 +2462,9 @@
         <v>821</v>
       </c>
     </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>SULGIPE</t>
-        </is>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>62</v>
       </c>
       <c r="B54">
         <v>127</v>
@@ -2375,11 +2497,9 @@
         <v>111</v>
       </c>
     </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>UHENPAL</t>
-        </is>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>63</v>
       </c>
       <c r="B55">
         <v>41</v>

</xml_diff>